<commit_message>
修改战斗相关逻辑 支持退出 Signed-off-by: xxp-pc-yanjiao <xxpniu@qq.com>
</commit_message>
<xml_diff>
--- a/ExcelConfig/地图表.xlsx
+++ b/ExcelConfig/地图表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="__Base" sheetId="2" r:id="rId1"/>
@@ -41,10 +41,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hero1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Int</t>
   </si>
   <si>
@@ -178,11 +174,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>1|2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>map1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>1|2</t>
+    <t>云栈洞</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -567,27 +567,27 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.77734375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.75" style="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" style="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -601,30 +601,30 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N12" sqref="N12"/>
+      <selection pane="bottomRight" activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.875" style="2" customWidth="1"/>
     <col min="3" max="3" width="9" style="2"/>
-    <col min="4" max="4" width="15.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.375" style="2" customWidth="1"/>
     <col min="7" max="8" width="9" style="2"/>
-    <col min="9" max="9" width="18.6640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="15.88671875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="18.625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="15.875" style="2" customWidth="1"/>
     <col min="11" max="13" width="9" style="2"/>
-    <col min="14" max="14" width="18.5546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="17.109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="18.5" style="2" customWidth="1"/>
+    <col min="15" max="15" width="17.125" style="2" customWidth="1"/>
     <col min="16" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -635,102 +635,102 @@
         <v>4</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="D2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="O2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="3" spans="1:17" ht="16.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
@@ -741,60 +741,60 @@
         <v>5</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="N3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="O4" s="2">
         <v>6000</v>

</xml_diff>